<commit_message>
Updated community profiles different sources excel sheet
</commit_message>
<xml_diff>
--- a/resources/community_profiles_different_sources.xlsx
+++ b/resources/community_profiles_different_sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christopher.smith\OneDrive - Cook County Health\git_repos\justenvirons\scc-community-profiles\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amder\Desktop\RA Github\scc-community-profiles\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{6E83DEBF-4B43-4C7F-8662-0F9F430311F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D620B841-1FB9-488B-BC36-1BEEF3B62B42}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{596BAAFF-C555-4844-B317-0EC167B2211B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4F50F19F-D296-4B9C-8CD4-875E928491F3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4F50F19F-D296-4B9C-8CD4-875E928491F3}"/>
   </bookViews>
   <sheets>
     <sheet name="profile assessment (transposed)" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="63">
   <si>
     <t>Category</t>
   </si>
@@ -183,13 +183,55 @@
   </si>
   <si>
     <t>Source4= America'sHealthRankings-Illinois- Explore Health Measures and Rankings in Illinois | AHR, for Data sources: https://www.americashealthrankings.org/learn/reports/2023-annual-report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source8= </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source9= </t>
+  </si>
+  <si>
+    <t>Source10+</t>
+  </si>
+  <si>
+    <t>Source5= NYC.gov Community Health Profiles</t>
+  </si>
+  <si>
+    <t>59 communites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t>Yes-languages &amp; font sizing</t>
+  </si>
+  <si>
+    <t>Source6= Department of Health &amp; Social Care Public Health Profiles (United Kingdom)</t>
+  </si>
+  <si>
+    <t>4 Area Types</t>
+  </si>
+  <si>
+    <t>7/38</t>
+  </si>
+  <si>
+    <t>Source7= Houston Health Department Community Health Profiles and Reports</t>
+  </si>
+  <si>
+    <t>4 Communities</t>
+  </si>
+  <si>
+    <t>3/20</t>
+  </si>
+  <si>
+    <t>Yes-Houston State of Health, CDC, Healthy People 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,10 +278,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -259,7 +304,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59A14D49-16A8-4E0F-943C-D2D58DE3E486}" name="Table1" displayName="Table1" ref="A1:L18" totalsRowShown="0">
-  <autoFilter ref="A1:L18" xr:uid="{59A14D49-16A8-4E0F-943C-D2D58DE3E486}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{9CAFA580-E19D-423D-8653-A3D6A7B4CAEE}" name="Category"/>
     <tableColumn id="2" xr3:uid="{B274464D-B572-4505-8E80-992A3BB4C1A6}" name="Attribute"/>
@@ -595,21 +639,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{626A8EBB-C25F-45F7-8A1A-22138D699762}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="9.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +699,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -666,8 +718,17 @@
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15">
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -686,8 +747,17 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="15">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -706,8 +776,17 @@
       <c r="F4" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="15">
+      <c r="G4">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -726,8 +805,17 @@
       <c r="F5" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="15">
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -746,8 +834,17 @@
       <c r="F6" s="1">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="15">
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -766,8 +863,17 @@
       <c r="F7" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="15">
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -786,8 +892,17 @@
       <c r="F8" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="15">
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -806,8 +921,17 @@
       <c r="F9" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="15">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -826,8 +950,17 @@
       <c r="F10" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="15">
+      <c r="G10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -846,8 +979,17 @@
       <c r="F11" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="15">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -864,8 +1006,14 @@
         <v>1</v>
       </c>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" ht="15">
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="I12">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -884,8 +1032,11 @@
       <c r="F13" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="15">
+      <c r="H13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -902,8 +1053,17 @@
       <c r="F14" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="15">
+      <c r="G14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H14" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -922,8 +1082,17 @@
       <c r="F15" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="15">
+      <c r="G15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" t="s">
+        <v>41</v>
+      </c>
+      <c r="I15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -942,8 +1111,17 @@
       <c r="F16" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="15">
+      <c r="G16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -960,8 +1138,17 @@
       <c r="F17" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="15">
+      <c r="G17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>42</v>
       </c>
@@ -976,32 +1163,72 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-    </row>
-    <row r="22" spans="1:6" ht="15">
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>